<commit_message>
Changed execution count in GSBD and GSBD2 notebooks, necessary for accurate tracking.
</commit_message>
<xml_diff>
--- a/GSBD/GSBC_sec_filing_links.xlsx
+++ b/GSBD/GSBC_sec_filing_links.xlsx
@@ -838,112 +838,112 @@
     <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312515186991/d904930d10q.htm</t>
   </si>
   <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-24-022198.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-23-060336.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-23-037958.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-23-017863.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-23-004160.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-22-021910.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-22-014734.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-22-007837.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0000950170-22-001971.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001564590-21-054478.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001564590-21-041640.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001564590-21-024971.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001564590-21-008932.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001564590-20-051458.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001564590-20-038967.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001564590-20-024262.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-20-043607.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-19-287306.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-19-210919.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-19-143069.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-19-057955.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-18-315859.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-18-236764.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-18-150950.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-18-054327.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-17-331120.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-17-247530.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-17-158958.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-17-062673.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-16-758892.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-16-671940.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-16-584019.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-16-490118.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-15-368460.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-15-280988.txt</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001572694/0001193125-15-186991.txt</t>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017024022198/0000950170-24-022198.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017023060336/0000950170-23-060336.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017023037958/0000950170-23-037958.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017023017863/0000950170-23-017863.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017023004160/0000950170-23-004160.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017022021910/0000950170-22-021910.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017022014734/0000950170-22-014734.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017022007837/0000950170-22-007837.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000095017022001971/0000950170-22-001971.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000156459021054478/0001564590-21-054478.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000156459021041640/0001564590-21-041640.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000156459021024971/0001564590-21-024971.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000156459021008932/0001564590-21-008932.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000156459020051458/0001564590-20-051458.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000156459020038967/0001564590-20-038967.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000156459020024262/0001564590-20-024262.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312520043607/0001193125-20-043607.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312519287306/0001193125-19-287306.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312519210919/0001193125-19-210919.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312519143069/0001193125-19-143069.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312519057955/0001193125-19-057955.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312518315859/0001193125-18-315859.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312518236764/0001193125-18-236764.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312518150950/0001193125-18-150950.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312518054327/0001193125-18-054327.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312517331120/0001193125-17-331120.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312517247530/0001193125-17-247530.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312517158958/0001193125-17-158958.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312517062673/0001193125-17-062673.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312516758892/0001193125-16-758892.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312516671940/0001193125-16-671940.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312516584019/0001193125-16-584019.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312516490118/0001193125-16-490118.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312515368460/0001193125-15-368460.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312515280988/0001193125-15-280988.txt</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/0001572694/000119312515186991/0001193125-15-186991.txt</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1333,7 @@
     <col min="13" max="13" width="23.7109375" customWidth="1"/>
     <col min="14" max="14" width="25.7109375" customWidth="1"/>
     <col min="15" max="15" width="93.7109375" customWidth="1"/>
-    <col min="16" max="16" width="77.7109375" customWidth="1"/>
+    <col min="16" max="16" width="96.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>